<commit_message>
Cleaned up for publication
</commit_message>
<xml_diff>
--- a/Microscopy_1.xlsx
+++ b/Microscopy_1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schlenge\LPBF-SmartAM-Optical-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masg\Documents\Papers\Processing_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28DC19B-785C-4454-8149-46A487275BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E7E40E48-3456-4DAD-98A5-89F0581674E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="11">
   <si>
     <t>Cube</t>
   </si>
@@ -74,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,16 +438,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83B8421-C040-4231-B330-906112788400}">
-  <dimension ref="A1:D101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -462,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -476,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -490,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -504,7 +503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -518,7 +517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -532,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -546,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -560,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -574,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -588,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -602,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -616,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -630,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -644,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -658,7 +657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -672,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -686,7 +685,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -700,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -714,7 +713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -728,7 +727,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -742,26 +741,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -770,12 +769,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -784,26 +783,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -812,26 +811,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -840,26 +839,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -868,12 +867,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -882,12 +881,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -896,12 +895,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -910,68 +909,68 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38">
         <v>7</v>
@@ -980,96 +979,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C39">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C40">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -1078,26 +1077,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C46">
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C47">
         <v>6</v>
@@ -1106,12 +1105,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>7</v>
@@ -1120,12 +1119,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C49">
         <v>8</v>
@@ -1134,26 +1133,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C51">
         <v>10</v>
@@ -1162,26 +1161,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B53">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -1190,26 +1189,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <v>4</v>
@@ -1218,12 +1217,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B56">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>5</v>
@@ -1232,26 +1231,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C57">
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B58">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <v>7</v>
@@ -1260,12 +1259,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B59">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C59">
         <v>8</v>
@@ -1274,12 +1273,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C60">
         <v>9</v>
@@ -1288,68 +1287,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B61">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C61">
         <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>4</v>
       </c>
       <c r="B62">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>4</v>
       </c>
       <c r="B64">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>4</v>
       </c>
       <c r="B65">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>4</v>
@@ -1358,40 +1357,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>4</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>4</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>4</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C68">
         <v>7</v>
@@ -1400,12 +1399,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>4</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>8</v>
@@ -1414,26 +1413,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>4</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C70">
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>4</v>
       </c>
       <c r="B71">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C71">
         <v>10</v>
@@ -1442,26 +1441,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>4</v>
       </c>
       <c r="B72">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>4</v>
       </c>
       <c r="B73">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -1470,12 +1469,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>4</v>
       </c>
       <c r="B74">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C74">
         <v>3</v>
@@ -1484,12 +1483,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <v>4</v>
@@ -1498,12 +1497,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>4</v>
       </c>
       <c r="B76">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C76">
         <v>5</v>
@@ -1512,40 +1511,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>4</v>
       </c>
       <c r="B77">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C77">
         <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>4</v>
       </c>
       <c r="B78">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C78">
         <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>4</v>
       </c>
       <c r="B79">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C79">
         <v>8</v>
@@ -1554,12 +1553,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>4</v>
       </c>
       <c r="B80">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C80">
         <v>9</v>
@@ -1568,12 +1567,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>4</v>
       </c>
       <c r="B81">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C81">
         <v>10</v>
@@ -1582,40 +1581,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>4</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>4</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C83">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>4</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -1624,40 +1623,40 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>4</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C85">
         <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>4</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C86">
         <v>5</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>4</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C87">
         <v>6</v>
@@ -1666,12 +1665,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>4</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C88">
         <v>7</v>
@@ -1680,26 +1679,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>4</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C89">
         <v>8</v>
       </c>
       <c r="D89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>4</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C90">
         <v>9</v>
@@ -1708,12 +1707,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>4</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C91">
         <v>10</v>
@@ -1722,26 +1721,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>4</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C92">
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>4</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -1750,40 +1749,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>4</v>
       </c>
       <c r="B94">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C94">
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>4</v>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C95">
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>4</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C96">
         <v>5</v>
@@ -1792,40 +1791,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>4</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C97">
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>4</v>
       </c>
       <c r="B98">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C98">
         <v>7</v>
       </c>
       <c r="D98" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>4</v>
       </c>
       <c r="B99">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C99">
         <v>8</v>
@@ -1834,31 +1833,311 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>4</v>
       </c>
       <c r="B100">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C100">
         <v>9</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>4</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C101">
         <v>10</v>
       </c>
       <c r="D101" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>1</v>
+      </c>
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+      <c r="C105">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106">
+        <v>1</v>
+      </c>
+      <c r="C106">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+      <c r="C109">
+        <v>8</v>
+      </c>
+      <c r="D109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="C116">
+        <v>5</v>
+      </c>
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+      <c r="C117">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="C118">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120">
+        <v>2</v>
+      </c>
+      <c r="C120">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>4</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+      <c r="C121">
+        <v>10</v>
+      </c>
+      <c r="D121" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>